<commit_message>
[update ppt và xlsx][lebatruc] - Cập nhật pptx
</commit_message>
<xml_diff>
--- a/Result_Demo.xlsx
+++ b/Result_Demo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LinhTinh\Master_Course\HK1\AnToanHeThongTin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF497931-2215-46AD-BADD-F53FCA8D0322}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{192F7872-96DC-4121-B864-B41B83BB8BCC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{0C6781A4-4849-4987-B97F-3F5D65182FC6}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="47">
   <si>
     <t>Train</t>
   </si>
@@ -171,6 +171,15 @@
   </si>
   <si>
     <t>Mean-Based Avagared</t>
+  </si>
+  <si>
+    <t>Số lượng</t>
+  </si>
+  <si>
+    <t>Phân phối</t>
+  </si>
+  <si>
+    <t>Label_encoded</t>
   </si>
 </sst>
 </file>
@@ -268,15 +277,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -292,9 +298,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -305,31 +308,40 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -665,862 +677,886 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE8C3FCA-59E7-49CA-A5BD-623315E3C813}">
-  <dimension ref="A1:M36"/>
+  <dimension ref="A1:M37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O8" sqref="O8"/>
+      <selection activeCell="U20" sqref="U20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.140625" customWidth="1"/>
-    <col min="3" max="3" width="9.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="8" width="9.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="11" width="9.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="23" t="s">
+      <c r="A1" s="20" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="23"/>
-      <c r="C1" s="23"/>
-      <c r="D1" s="23"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
+      <c r="B1" s="20"/>
+      <c r="C1" s="20"/>
+      <c r="D1" s="20"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+      <c r="I1" s="14"/>
+      <c r="J1" s="14"/>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="18" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="D2" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="14"/>
+      <c r="J2" s="14"/>
+      <c r="K2" s="14"/>
+      <c r="L2" s="14"/>
+      <c r="M2" s="14"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B3" s="15">
         <v>358332</v>
       </c>
-      <c r="C2" s="21">
+      <c r="C3" s="16">
         <v>0.8</v>
       </c>
-      <c r="D2" s="22">
-        <v>0</v>
-      </c>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="19"/>
-      <c r="I2" s="19"/>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="20" t="s">
+      <c r="D3" s="17">
+        <v>0</v>
+      </c>
+      <c r="E3" s="14"/>
+      <c r="F3" s="14"/>
+      <c r="G3" s="14"/>
+      <c r="H3" s="14"/>
+      <c r="I3" s="14"/>
+      <c r="J3" s="14"/>
+      <c r="K3" s="14"/>
+      <c r="L3" s="14"/>
+      <c r="M3" s="14"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="20">
+      <c r="B4" s="15">
         <v>30951</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C4" s="16">
         <v>6.9099999999999995E-2</v>
       </c>
-      <c r="D3" s="22">
+      <c r="D4" s="17">
         <v>4</v>
       </c>
-      <c r="E3" s="19"/>
-      <c r="F3" s="19"/>
-      <c r="G3" s="19"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="19"/>
-      <c r="J3" s="19"/>
-      <c r="K3" s="19"/>
-      <c r="L3" s="19"/>
-      <c r="M3" s="19"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="20" t="s">
+      <c r="E4" s="14"/>
+      <c r="F4" s="14"/>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14"/>
+      <c r="K4" s="14"/>
+      <c r="L4" s="14"/>
+      <c r="M4" s="14"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B5" s="15">
         <v>29613</v>
       </c>
-      <c r="C4" s="21">
+      <c r="C5" s="16">
         <v>6.6113000000000005E-2</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D5" s="17">
         <v>5</v>
       </c>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A5" s="20" t="s">
+      <c r="E5" s="14"/>
+      <c r="F5" s="14"/>
+      <c r="G5" s="14"/>
+      <c r="H5" s="14"/>
+      <c r="I5" s="14"/>
+      <c r="J5" s="14"/>
+      <c r="K5" s="14"/>
+      <c r="L5" s="14"/>
+      <c r="M5" s="14"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="20">
+      <c r="B6" s="15">
         <v>16735</v>
       </c>
-      <c r="C5" s="21">
+      <c r="C6" s="16">
         <v>3.7361999999999999E-2</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D6" s="17">
         <v>7</v>
       </c>
-      <c r="E5" s="19"/>
-      <c r="F5" s="19"/>
-      <c r="G5" s="19"/>
-      <c r="H5" s="19"/>
-      <c r="I5" s="19"/>
-      <c r="J5" s="19"/>
-      <c r="K5" s="19"/>
-      <c r="L5" s="19"/>
-      <c r="M5" s="19"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="20" t="s">
+      <c r="E6" s="14"/>
+      <c r="F6" s="14"/>
+      <c r="G6" s="14"/>
+      <c r="H6" s="14"/>
+      <c r="I6" s="14"/>
+      <c r="J6" s="14"/>
+      <c r="K6" s="14"/>
+      <c r="L6" s="14"/>
+      <c r="M6" s="14"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="20">
+      <c r="B7" s="15">
         <v>4632</v>
       </c>
-      <c r="C6" s="21">
+      <c r="C7" s="16">
         <v>1.0340999999999999E-2</v>
       </c>
-      <c r="D6" s="22">
+      <c r="D7" s="17">
         <v>6</v>
       </c>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="19"/>
-      <c r="H6" s="19"/>
-      <c r="I6" s="19"/>
-      <c r="J6" s="19"/>
-      <c r="K6" s="19"/>
-      <c r="L6" s="19"/>
-      <c r="M6" s="19"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="20" t="s">
+      <c r="E7" s="14"/>
+      <c r="F7" s="14"/>
+      <c r="G7" s="14"/>
+      <c r="H7" s="14"/>
+      <c r="I7" s="14"/>
+      <c r="J7" s="14"/>
+      <c r="K7" s="14"/>
+      <c r="L7" s="14"/>
+      <c r="M7" s="14"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="20">
+      <c r="B8" s="15">
         <v>4467</v>
       </c>
-      <c r="C7" s="21">
+      <c r="C8" s="16">
         <v>9.9729999999999992E-3</v>
       </c>
-      <c r="D7" s="22">
+      <c r="D8" s="17">
         <v>3</v>
       </c>
-      <c r="E7" s="19"/>
-      <c r="F7" s="19"/>
-      <c r="G7" s="19"/>
-      <c r="H7" s="19"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="19"/>
-      <c r="K7" s="19"/>
-      <c r="L7" s="19"/>
-      <c r="M7" s="19"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="20" t="s">
+      <c r="E8" s="14"/>
+      <c r="F8" s="14"/>
+      <c r="G8" s="14"/>
+      <c r="H8" s="14"/>
+      <c r="I8" s="14"/>
+      <c r="J8" s="14"/>
+      <c r="K8" s="14"/>
+      <c r="L8" s="14"/>
+      <c r="M8" s="14"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="B8" s="20">
+      <c r="B9" s="15">
         <v>2102</v>
       </c>
-      <c r="C8" s="21">
+      <c r="C9" s="16">
         <v>4.6930000000000001E-3</v>
       </c>
-      <c r="D8" s="22">
+      <c r="D9" s="17">
         <v>8</v>
       </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="20" t="s">
+      <c r="E9" s="14"/>
+      <c r="F9" s="14"/>
+      <c r="G9" s="14"/>
+      <c r="H9" s="14"/>
+      <c r="I9" s="14"/>
+      <c r="J9" s="14"/>
+      <c r="K9" s="14"/>
+      <c r="L9" s="14"/>
+      <c r="M9" s="14"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="B9" s="20">
+      <c r="B10" s="15">
         <v>452</v>
       </c>
-      <c r="C9" s="21">
+      <c r="C10" s="16">
         <v>1.0089999999999999E-3</v>
       </c>
-      <c r="D9" s="22">
+      <c r="D10" s="17">
         <v>2</v>
       </c>
-      <c r="E9" s="19"/>
-      <c r="F9" s="19"/>
-      <c r="G9" s="19"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="19"/>
-      <c r="J9" s="19"/>
-      <c r="K9" s="19"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="19"/>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A10" s="20" t="s">
+      <c r="E10" s="14"/>
+      <c r="F10" s="14"/>
+      <c r="G10" s="14"/>
+      <c r="H10" s="14"/>
+      <c r="I10" s="14"/>
+      <c r="J10" s="14"/>
+      <c r="K10" s="14"/>
+      <c r="L10" s="14"/>
+      <c r="M10" s="14"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="B10" s="20">
+      <c r="B11" s="15">
         <v>385</v>
       </c>
-      <c r="C10" s="21">
+      <c r="C11" s="16">
         <v>8.5999999999999998E-4</v>
       </c>
-      <c r="D10" s="22">
+      <c r="D11" s="17">
         <v>1</v>
       </c>
-      <c r="E10" s="19"/>
-      <c r="F10" s="19"/>
-      <c r="G10" s="19"/>
-      <c r="H10" s="19"/>
-      <c r="I10" s="19"/>
-      <c r="J10" s="19"/>
-      <c r="K10" s="19"/>
-      <c r="L10" s="19"/>
-      <c r="M10" s="19"/>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A11" s="20" t="s">
+      <c r="E11" s="14"/>
+      <c r="F11" s="14"/>
+      <c r="G11" s="14"/>
+      <c r="H11" s="14"/>
+      <c r="I11" s="14"/>
+      <c r="J11" s="14"/>
+      <c r="K11" s="14"/>
+      <c r="L11" s="14"/>
+      <c r="M11" s="14"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="B11" s="20">
+      <c r="B12" s="15">
         <v>246</v>
       </c>
-      <c r="C11" s="21">
+      <c r="C12" s="16">
         <v>5.4900000000000001E-4</v>
       </c>
-      <c r="D11" s="22">
+      <c r="D12" s="17">
         <v>9</v>
       </c>
-      <c r="E11" s="19"/>
-      <c r="F11" s="19"/>
-      <c r="G11" s="19"/>
-      <c r="H11" s="19"/>
-      <c r="I11" s="19"/>
-      <c r="J11" s="19"/>
-      <c r="K11" s="19"/>
-      <c r="L11" s="19"/>
-      <c r="M11" s="19"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
-      <c r="B12" s="19"/>
-      <c r="C12" s="19"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="19"/>
-      <c r="G12" s="19"/>
-      <c r="H12" s="19"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="19"/>
-      <c r="K12" s="19"/>
-      <c r="L12" s="19"/>
-      <c r="M12" s="19"/>
+      <c r="E12" s="14"/>
+      <c r="F12" s="14"/>
+      <c r="G12" s="14"/>
+      <c r="H12" s="14"/>
+      <c r="I12" s="14"/>
+      <c r="J12" s="14"/>
+      <c r="K12" s="14"/>
+      <c r="L12" s="14"/>
+      <c r="M12" s="14"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13" s="18"/>
-      <c r="C13" s="19"/>
-      <c r="D13" s="18" t="s">
+      <c r="A13" s="14"/>
+      <c r="B13" s="14"/>
+      <c r="C13" s="14"/>
+      <c r="D13" s="14"/>
+      <c r="E13" s="14"/>
+      <c r="F13" s="14"/>
+      <c r="G13" s="14"/>
+      <c r="H13" s="14"/>
+      <c r="I13" s="14"/>
+      <c r="J13" s="14"/>
+      <c r="K13" s="14"/>
+      <c r="L13" s="14"/>
+      <c r="M13" s="14"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14" s="19"/>
+      <c r="C14" s="14"/>
+      <c r="D14" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="E13" s="18"/>
-      <c r="F13" s="19"/>
-      <c r="G13" s="18" t="s">
+      <c r="E14" s="19"/>
+      <c r="F14" s="14"/>
+      <c r="G14" s="19" t="s">
         <v>2</v>
       </c>
-      <c r="H13" s="18"/>
-      <c r="I13" s="19"/>
-      <c r="J13" s="18" t="s">
+      <c r="H14" s="19"/>
+      <c r="I14" s="14"/>
+      <c r="J14" s="19" t="s">
         <v>3</v>
       </c>
-      <c r="K13" s="18"/>
-      <c r="L13" s="19"/>
-      <c r="M13" s="19"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>0</v>
-      </c>
-      <c r="B14" s="3">
+      <c r="K14" s="19"/>
+      <c r="L14" s="14"/>
+      <c r="M14" s="14"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>0</v>
+      </c>
+      <c r="B15" s="2">
         <v>286741</v>
       </c>
-      <c r="C14" s="19"/>
-      <c r="D14" s="2">
-        <v>0</v>
-      </c>
-      <c r="E14" s="3">
+      <c r="C15" s="14"/>
+      <c r="D15" s="1">
+        <v>0</v>
+      </c>
+      <c r="E15" s="2">
         <v>143143</v>
       </c>
-      <c r="F14" s="19"/>
-      <c r="G14" s="2">
-        <v>0</v>
-      </c>
-      <c r="H14" s="3">
+      <c r="F15" s="14"/>
+      <c r="G15" s="1">
+        <v>0</v>
+      </c>
+      <c r="H15" s="2">
         <v>143368</v>
       </c>
-      <c r="I14" s="19"/>
-      <c r="J14" s="2">
-        <v>0</v>
-      </c>
-      <c r="K14" s="3">
+      <c r="I15" s="14"/>
+      <c r="J15" s="1">
+        <v>0</v>
+      </c>
+      <c r="K15" s="2">
         <v>143351</v>
       </c>
-      <c r="L14" s="19"/>
-      <c r="M14" s="19"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+      <c r="L15" s="14"/>
+      <c r="M15" s="14"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
         <v>4</v>
       </c>
-      <c r="B15" s="3">
+      <c r="B16" s="2">
         <v>24714</v>
       </c>
-      <c r="C15" s="19"/>
-      <c r="D15" s="2">
+      <c r="C16" s="14"/>
+      <c r="D16" s="1">
         <v>5</v>
       </c>
-      <c r="E15" s="3">
+      <c r="E16" s="2">
         <v>11925</v>
       </c>
-      <c r="F15" s="19"/>
-      <c r="G15" s="2">
+      <c r="F16" s="14"/>
+      <c r="G16" s="1">
         <v>5</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H16" s="2">
         <v>11816</v>
       </c>
-      <c r="I15" s="19"/>
-      <c r="J15" s="2">
+      <c r="I16" s="14"/>
+      <c r="J16" s="1">
         <v>7</v>
       </c>
-      <c r="K15" s="3">
+      <c r="K16" s="2">
         <v>13393</v>
       </c>
-      <c r="L15" s="19"/>
-      <c r="M15" s="19"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+      <c r="L16" s="14"/>
+      <c r="M16" s="14"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
         <v>5</v>
       </c>
-      <c r="B16" s="3">
+      <c r="B17" s="2">
         <v>23605</v>
       </c>
-      <c r="C16" s="19"/>
-      <c r="D16" s="2">
+      <c r="C17" s="14"/>
+      <c r="D17" s="1">
         <v>7</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E17" s="2">
         <v>6744</v>
       </c>
-      <c r="F16" s="19"/>
-      <c r="G16" s="2">
+      <c r="F17" s="14"/>
+      <c r="G17" s="1">
         <v>7</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H17" s="2">
         <v>6635</v>
       </c>
-      <c r="I16" s="19"/>
-      <c r="J16" s="16">
+      <c r="I17" s="14"/>
+      <c r="J17" s="12">
         <v>4</v>
       </c>
-      <c r="K16" s="17">
+      <c r="K17" s="13">
         <v>24839</v>
       </c>
-      <c r="L16" s="19"/>
-      <c r="M16" s="19"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
+      <c r="L17" s="14"/>
+      <c r="M17" s="14"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
         <v>7</v>
       </c>
-      <c r="B17" s="3">
+      <c r="B18" s="2">
         <v>13393</v>
       </c>
-      <c r="C17" s="19"/>
-      <c r="D17" s="2">
+      <c r="C18" s="14"/>
+      <c r="D18" s="1">
         <v>6</v>
       </c>
-      <c r="E17" s="3">
+      <c r="E18" s="2">
         <v>1878</v>
       </c>
-      <c r="F17" s="19"/>
-      <c r="G17" s="2">
+      <c r="F18" s="14"/>
+      <c r="G18" s="1">
         <v>6</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H18" s="2">
         <v>1872</v>
       </c>
-      <c r="I17" s="19"/>
-      <c r="J17" s="2">
+      <c r="I18" s="14"/>
+      <c r="J18" s="1">
         <v>5</v>
       </c>
-      <c r="K17" s="3">
+      <c r="K18" s="2">
         <v>11903</v>
       </c>
-      <c r="L17" s="19"/>
-      <c r="M17" s="19"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
+      <c r="L18" s="14"/>
+      <c r="M18" s="14"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
         <v>6</v>
       </c>
-      <c r="B18" s="3">
+      <c r="B19" s="2">
         <v>3720</v>
       </c>
-      <c r="C18" s="19"/>
-      <c r="D18" s="2">
+      <c r="C19" s="14"/>
+      <c r="D19" s="1">
         <v>3</v>
       </c>
-      <c r="E18" s="3">
+      <c r="E19" s="2">
         <v>1794</v>
       </c>
-      <c r="F18" s="19"/>
-      <c r="G18" s="2">
+      <c r="F19" s="14"/>
+      <c r="G19" s="1">
         <v>3</v>
       </c>
-      <c r="H18" s="3">
+      <c r="H19" s="2">
         <v>1797</v>
       </c>
-      <c r="I18" s="19"/>
-      <c r="J18" s="2">
+      <c r="I19" s="14"/>
+      <c r="J19" s="1">
         <v>6</v>
       </c>
-      <c r="K18" s="3">
+      <c r="K19" s="2">
         <v>1874</v>
       </c>
-      <c r="L18" s="19"/>
-      <c r="M18" s="19"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
+      <c r="L19" s="14"/>
+      <c r="M19" s="14"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
         <v>3</v>
       </c>
-      <c r="B19" s="3">
+      <c r="B20" s="2">
         <v>3596</v>
       </c>
-      <c r="C19" s="19"/>
-      <c r="D19" s="2">
+      <c r="C20" s="14"/>
+      <c r="D20" s="1">
         <v>8</v>
       </c>
-      <c r="E19" s="3">
+      <c r="E20" s="2">
         <v>854</v>
       </c>
-      <c r="F19" s="19"/>
-      <c r="G19" s="2">
+      <c r="F20" s="14"/>
+      <c r="G20" s="1">
         <v>8</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H20" s="2">
         <v>815</v>
       </c>
-      <c r="I19" s="19"/>
-      <c r="J19" s="2">
+      <c r="I20" s="14"/>
+      <c r="J20" s="1">
         <v>3</v>
       </c>
-      <c r="K19" s="3">
+      <c r="K20" s="2">
         <v>1802</v>
       </c>
-      <c r="L19" s="19"/>
-      <c r="M19" s="19"/>
-    </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
+      <c r="L20" s="14"/>
+      <c r="M20" s="14"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
         <v>8</v>
       </c>
-      <c r="B20" s="3">
+      <c r="B21" s="2">
         <v>1689</v>
       </c>
-      <c r="C20" s="19"/>
-      <c r="D20" s="2">
+      <c r="C21" s="14"/>
+      <c r="D21" s="1">
         <v>2</v>
       </c>
-      <c r="E20" s="3">
+      <c r="E21" s="2">
         <v>175</v>
       </c>
-      <c r="F20" s="19"/>
-      <c r="G20" s="2">
+      <c r="F21" s="14"/>
+      <c r="G21" s="1">
         <v>2</v>
       </c>
-      <c r="H20" s="3">
+      <c r="H21" s="2">
         <v>176</v>
       </c>
-      <c r="I20" s="19"/>
-      <c r="J20" s="2">
+      <c r="I21" s="14"/>
+      <c r="J21" s="1">
         <v>8</v>
       </c>
-      <c r="K20" s="3">
+      <c r="K21" s="2">
         <v>835</v>
       </c>
-      <c r="L20" s="19"/>
-      <c r="M20" s="19"/>
-    </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
+      <c r="L21" s="14"/>
+      <c r="M21" s="14"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
         <v>2</v>
       </c>
-      <c r="B21" s="3">
+      <c r="B22" s="2">
         <v>362</v>
       </c>
-      <c r="C21" s="19"/>
-      <c r="D21" s="2">
+      <c r="C22" s="14"/>
+      <c r="D22" s="1">
         <v>1</v>
       </c>
-      <c r="E21" s="3">
+      <c r="E22" s="2">
         <v>139</v>
       </c>
-      <c r="F21" s="19"/>
-      <c r="G21" s="2">
+      <c r="F22" s="14"/>
+      <c r="G22" s="1">
         <v>1</v>
       </c>
-      <c r="H21" s="3">
+      <c r="H22" s="2">
         <v>164</v>
       </c>
-      <c r="I21" s="19"/>
-      <c r="J21" s="2">
+      <c r="I22" s="14"/>
+      <c r="J22" s="1">
         <v>2</v>
       </c>
-      <c r="K21" s="3">
+      <c r="K22" s="2">
         <v>191</v>
       </c>
-      <c r="L21" s="19"/>
-      <c r="M21" s="19"/>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
+      <c r="L22" s="14"/>
+      <c r="M22" s="14"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
         <v>1</v>
       </c>
-      <c r="B22" s="3">
+      <c r="B23" s="2">
         <v>310</v>
       </c>
-      <c r="C22" s="19"/>
-      <c r="D22" s="2">
+      <c r="C23" s="14"/>
+      <c r="D23" s="1">
         <v>9</v>
       </c>
-      <c r="E22" s="3">
+      <c r="E23" s="2">
         <v>94</v>
       </c>
-      <c r="F22" s="19"/>
-      <c r="G22" s="2">
+      <c r="F23" s="14"/>
+      <c r="G23" s="1">
         <v>9</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H23" s="2">
         <v>104</v>
       </c>
-      <c r="I22" s="19"/>
-      <c r="J22" s="2">
+      <c r="I23" s="14"/>
+      <c r="J23" s="1">
         <v>1</v>
       </c>
-      <c r="K22" s="3">
+      <c r="K23" s="2">
         <v>136</v>
       </c>
-      <c r="L22" s="19"/>
-      <c r="M22" s="19"/>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
+      <c r="L23" s="14"/>
+      <c r="M23" s="14"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
         <v>9</v>
       </c>
-      <c r="B23" s="3">
+      <c r="B24" s="2">
         <v>202</v>
       </c>
-      <c r="C23" s="19"/>
-      <c r="D23" s="16">
+      <c r="C24" s="14"/>
+      <c r="D24" s="12">
         <v>4</v>
       </c>
-      <c r="E23" s="17">
-        <v>0</v>
-      </c>
-      <c r="F23" s="19"/>
-      <c r="G23" s="16">
+      <c r="E24" s="13">
+        <v>0</v>
+      </c>
+      <c r="F24" s="14"/>
+      <c r="G24" s="12">
         <v>4</v>
       </c>
-      <c r="H23" s="17">
-        <v>0</v>
-      </c>
-      <c r="I23" s="19"/>
-      <c r="J23" s="2">
+      <c r="H24" s="13">
+        <v>0</v>
+      </c>
+      <c r="I24" s="14"/>
+      <c r="J24" s="1">
         <v>9</v>
       </c>
-      <c r="K23" s="3">
+      <c r="K24" s="2">
         <v>107</v>
       </c>
-      <c r="L23" s="19"/>
-      <c r="M23" s="19"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A24" s="19"/>
-      <c r="B24" s="19"/>
-      <c r="C24" s="19"/>
-      <c r="D24" s="19"/>
-      <c r="E24" s="19"/>
-      <c r="F24" s="19"/>
-      <c r="G24" s="19"/>
-      <c r="H24" s="19"/>
-      <c r="I24" s="19"/>
-      <c r="J24" s="19"/>
-      <c r="K24" s="19"/>
-      <c r="L24" s="19"/>
-      <c r="M24" s="19"/>
+      <c r="L24" s="14"/>
+      <c r="M24" s="14"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A25" s="18" t="s">
+      <c r="A25" s="14"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="14"/>
+      <c r="D25" s="14"/>
+      <c r="E25" s="14"/>
+      <c r="F25" s="14"/>
+      <c r="G25" s="14"/>
+      <c r="H25" s="14"/>
+      <c r="I25" s="14"/>
+      <c r="J25" s="14"/>
+      <c r="K25" s="14"/>
+      <c r="L25" s="14"/>
+      <c r="M25" s="14"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="19" t="s">
         <v>4</v>
       </c>
-      <c r="B25" s="18"/>
-      <c r="C25" s="19"/>
-      <c r="D25" s="19"/>
-      <c r="E25" s="19"/>
-      <c r="F25" s="19"/>
-      <c r="G25" s="19"/>
-      <c r="H25" s="19"/>
-      <c r="I25" s="19"/>
-      <c r="J25" s="19"/>
-      <c r="K25" s="19"/>
-      <c r="L25" s="19"/>
-      <c r="M25" s="19"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>0</v>
-      </c>
-      <c r="B26" s="3">
+      <c r="B26" s="19"/>
+      <c r="C26" s="14"/>
+      <c r="D26" s="14"/>
+      <c r="E26" s="14"/>
+      <c r="F26" s="14"/>
+      <c r="G26" s="14"/>
+      <c r="H26" s="14"/>
+      <c r="I26" s="14"/>
+      <c r="J26" s="14"/>
+      <c r="K26" s="14"/>
+      <c r="L26" s="14"/>
+      <c r="M26" s="14"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="1">
+        <v>0</v>
+      </c>
+      <c r="B27" s="2">
         <v>71821</v>
       </c>
-      <c r="C26" s="19"/>
-      <c r="D26" s="19"/>
-      <c r="E26" s="19"/>
-      <c r="F26" s="19"/>
-      <c r="G26" s="19"/>
-      <c r="H26" s="19"/>
-      <c r="I26" s="19"/>
-      <c r="J26" s="19"/>
-      <c r="K26" s="19"/>
-      <c r="L26" s="19"/>
-      <c r="M26" s="19"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A27" s="16">
+      <c r="C27" s="14"/>
+      <c r="D27" s="14"/>
+      <c r="E27" s="14"/>
+      <c r="F27" s="14"/>
+      <c r="G27" s="14"/>
+      <c r="H27" s="14"/>
+      <c r="I27" s="14"/>
+      <c r="J27" s="14"/>
+      <c r="K27" s="14"/>
+      <c r="L27" s="14"/>
+      <c r="M27" s="14"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="12">
         <v>4</v>
       </c>
-      <c r="B27" s="17">
+      <c r="B28" s="13">
         <v>6112</v>
       </c>
-      <c r="C27" s="19"/>
-      <c r="D27" s="19"/>
-      <c r="E27" s="19"/>
-      <c r="F27" s="19"/>
-      <c r="G27" s="19"/>
-      <c r="H27" s="19"/>
-      <c r="I27" s="19"/>
-      <c r="J27" s="19"/>
-      <c r="K27" s="19"/>
-      <c r="L27" s="19"/>
-      <c r="M27" s="19"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
+      <c r="C28" s="14"/>
+      <c r="D28" s="14"/>
+      <c r="E28" s="14"/>
+      <c r="F28" s="14"/>
+      <c r="G28" s="14"/>
+      <c r="H28" s="14"/>
+      <c r="I28" s="14"/>
+      <c r="J28" s="14"/>
+      <c r="K28" s="14"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="14"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="1">
         <v>5</v>
       </c>
-      <c r="B28" s="3">
+      <c r="B29" s="2">
         <v>5872</v>
       </c>
-      <c r="C28" s="19"/>
-      <c r="D28" s="19"/>
-      <c r="E28" s="19"/>
-      <c r="F28" s="19"/>
-      <c r="G28" s="19"/>
-      <c r="H28" s="19"/>
-      <c r="I28" s="19"/>
-      <c r="J28" s="19"/>
-      <c r="K28" s="19"/>
-      <c r="L28" s="19"/>
-      <c r="M28" s="19"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
+      <c r="C29" s="14"/>
+      <c r="D29" s="14"/>
+      <c r="E29" s="14"/>
+      <c r="F29" s="14"/>
+      <c r="G29" s="14"/>
+      <c r="H29" s="14"/>
+      <c r="I29" s="14"/>
+      <c r="J29" s="14"/>
+      <c r="K29" s="14"/>
+      <c r="L29" s="14"/>
+      <c r="M29" s="14"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="1">
         <v>7</v>
       </c>
-      <c r="B29" s="3">
+      <c r="B30" s="2">
         <v>3356</v>
       </c>
-      <c r="C29" s="19"/>
-      <c r="D29" s="19"/>
-      <c r="E29" s="19"/>
-      <c r="F29" s="19"/>
-      <c r="G29" s="19"/>
-      <c r="H29" s="19"/>
-      <c r="I29" s="19"/>
-      <c r="J29" s="19"/>
-      <c r="K29" s="19"/>
-      <c r="L29" s="19"/>
-      <c r="M29" s="19"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
+      <c r="C30" s="14"/>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="14"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="1">
         <v>6</v>
       </c>
-      <c r="B30" s="3">
+      <c r="B31" s="2">
         <v>882</v>
       </c>
-      <c r="C30" s="19"/>
-      <c r="D30" s="19"/>
-      <c r="E30" s="19"/>
-      <c r="F30" s="19"/>
-      <c r="G30" s="19"/>
-      <c r="H30" s="19"/>
-      <c r="I30" s="19"/>
-      <c r="J30" s="19"/>
-      <c r="K30" s="19"/>
-      <c r="L30" s="19"/>
-      <c r="M30" s="19"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
+      <c r="C31" s="14"/>
+      <c r="D31" s="14"/>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="14"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="14"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="1">
         <v>3</v>
       </c>
-      <c r="B31" s="3">
+      <c r="B32" s="2">
         <v>876</v>
       </c>
-      <c r="C31" s="19"/>
-      <c r="D31" s="19"/>
-      <c r="E31" s="19"/>
-      <c r="F31" s="19"/>
-      <c r="G31" s="19"/>
-      <c r="H31" s="19"/>
-      <c r="I31" s="19"/>
-      <c r="J31" s="19"/>
-      <c r="K31" s="19"/>
-      <c r="L31" s="19"/>
-      <c r="M31" s="19"/>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A32" s="2">
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="14"/>
+      <c r="H32" s="14"/>
+      <c r="I32" s="14"/>
+      <c r="J32" s="14"/>
+      <c r="K32" s="14"/>
+      <c r="L32" s="14"/>
+      <c r="M32" s="14"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="1">
         <v>8</v>
       </c>
-      <c r="B32" s="3">
+      <c r="B33" s="2">
         <v>433</v>
       </c>
-      <c r="C32" s="19"/>
-      <c r="D32" s="19"/>
-      <c r="E32" s="19"/>
-      <c r="F32" s="19"/>
-      <c r="G32" s="19"/>
-      <c r="H32" s="19"/>
-      <c r="I32" s="19"/>
-      <c r="J32" s="19"/>
-      <c r="K32" s="19"/>
-      <c r="L32" s="19"/>
-      <c r="M32" s="19"/>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A33" s="2">
+      <c r="C33" s="14"/>
+      <c r="D33" s="14"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="14"/>
+      <c r="G33" s="14"/>
+      <c r="H33" s="14"/>
+      <c r="I33" s="14"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="14"/>
+      <c r="L33" s="14"/>
+      <c r="M33" s="14"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="1">
         <v>2</v>
       </c>
-      <c r="B33" s="3">
+      <c r="B34" s="2">
         <v>101</v>
       </c>
-      <c r="C33" s="19"/>
-      <c r="D33" s="19"/>
-      <c r="E33" s="19"/>
-      <c r="F33" s="19"/>
-      <c r="G33" s="19"/>
-      <c r="H33" s="19"/>
-      <c r="I33" s="19"/>
-      <c r="J33" s="19"/>
-      <c r="K33" s="19"/>
-      <c r="L33" s="19"/>
-      <c r="M33" s="19"/>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A34" s="2">
+      <c r="C34" s="14"/>
+      <c r="D34" s="14"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="14"/>
+      <c r="G34" s="14"/>
+      <c r="H34" s="14"/>
+      <c r="I34" s="14"/>
+      <c r="J34" s="14"/>
+      <c r="K34" s="14"/>
+      <c r="L34" s="14"/>
+      <c r="M34" s="14"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="1">
         <v>1</v>
       </c>
-      <c r="B34" s="3">
+      <c r="B35" s="2">
         <v>82</v>
       </c>
-      <c r="C34" s="19"/>
-      <c r="D34" s="19"/>
-      <c r="E34" s="19"/>
-      <c r="F34" s="19"/>
-      <c r="G34" s="19"/>
-      <c r="H34" s="19"/>
-      <c r="I34" s="19"/>
-      <c r="J34" s="19"/>
-      <c r="K34" s="19"/>
-      <c r="L34" s="19"/>
-      <c r="M34" s="19"/>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A35" s="2">
+      <c r="C35" s="14"/>
+      <c r="D35" s="14"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14"/>
+      <c r="G35" s="14"/>
+      <c r="H35" s="14"/>
+      <c r="I35" s="14"/>
+      <c r="J35" s="14"/>
+      <c r="K35" s="14"/>
+      <c r="L35" s="14"/>
+      <c r="M35" s="14"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="1">
         <v>9</v>
       </c>
-      <c r="B35" s="3">
+      <c r="B36" s="2">
         <v>48</v>
       </c>
-      <c r="C35" s="19"/>
-      <c r="D35" s="19"/>
-      <c r="E35" s="19"/>
-      <c r="F35" s="19"/>
-      <c r="G35" s="19"/>
-      <c r="H35" s="19"/>
-      <c r="I35" s="19"/>
-      <c r="J35" s="19"/>
-      <c r="K35" s="19"/>
-      <c r="L35" s="19"/>
-      <c r="M35" s="19"/>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A36" s="19"/>
-      <c r="B36" s="19"/>
-      <c r="C36" s="19"/>
-      <c r="D36" s="19"/>
-      <c r="E36" s="19"/>
-      <c r="F36" s="19"/>
-      <c r="G36" s="19"/>
-      <c r="H36" s="19"/>
-      <c r="I36" s="19"/>
-      <c r="J36" s="19"/>
-      <c r="K36" s="19"/>
-      <c r="L36" s="19"/>
-      <c r="M36" s="19"/>
+      <c r="C36" s="14"/>
+      <c r="D36" s="14"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="14"/>
+      <c r="G36" s="14"/>
+      <c r="H36" s="14"/>
+      <c r="I36" s="14"/>
+      <c r="J36" s="14"/>
+      <c r="K36" s="14"/>
+      <c r="L36" s="14"/>
+      <c r="M36" s="14"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="14"/>
+      <c r="B37" s="14"/>
+      <c r="C37" s="14"/>
+      <c r="D37" s="14"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="14"/>
+      <c r="G37" s="14"/>
+      <c r="H37" s="14"/>
+      <c r="I37" s="14"/>
+      <c r="J37" s="14"/>
+      <c r="K37" s="14"/>
+      <c r="L37" s="14"/>
+      <c r="M37" s="14"/>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="D13:E13"/>
-    <mergeCell ref="G13:H13"/>
-    <mergeCell ref="J13:K13"/>
-    <mergeCell ref="A25:B25"/>
     <mergeCell ref="A1:D1"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="A26:B26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1541,492 +1577,492 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="I1" s="1" t="s">
+      <c r="B1" s="21"/>
+      <c r="C1" s="21"/>
+      <c r="D1" s="21"/>
+      <c r="E1" s="21"/>
+      <c r="F1" s="21"/>
+      <c r="I1" s="21" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
-      <c r="M1" s="1"/>
+      <c r="J1" s="21"/>
+      <c r="K1" s="21"/>
+      <c r="L1" s="21"/>
+      <c r="M1" s="21"/>
     </row>
     <row r="2" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>0.99</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>0.97</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>0.98</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="8">
         <v>71821</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="I3" s="6" t="s">
+      <c r="F3" s="5"/>
+      <c r="I3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="5">
         <v>0.99</v>
       </c>
-      <c r="K3" s="6">
+      <c r="K3" s="5">
         <v>0.97</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L3" s="5">
         <v>0.98</v>
       </c>
-      <c r="M3" s="10">
+      <c r="M3" s="8">
         <v>71603</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="6">
+      <c r="B4" s="5">
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="5">
         <v>0.01</v>
       </c>
-      <c r="D4" s="6">
+      <c r="D4" s="5">
         <v>0.02</v>
       </c>
-      <c r="E4" s="6">
+      <c r="E4" s="5">
         <v>82</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="I4" s="6" t="s">
+      <c r="F4" s="5"/>
+      <c r="I4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="J4" s="6">
+      <c r="J4" s="5">
         <v>0.26</v>
       </c>
-      <c r="K4" s="6">
+      <c r="K4" s="5">
         <v>0.11</v>
       </c>
-      <c r="L4" s="6">
+      <c r="L4" s="5">
         <v>0.15</v>
       </c>
-      <c r="M4" s="6">
+      <c r="M4" s="5">
         <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>0.8</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>0.08</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>0.14000000000000001</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>101</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="I5" s="6" t="s">
+      <c r="F5" s="5"/>
+      <c r="I5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="5">
         <v>0.5</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="5">
         <v>0.01</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L5" s="5">
         <v>0.02</v>
       </c>
-      <c r="M5" s="6">
+      <c r="M5" s="5">
         <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>0.1</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>0.31</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>0.15</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>876</v>
       </c>
-      <c r="F6" s="6"/>
-      <c r="I6" s="6" t="s">
+      <c r="F6" s="5"/>
+      <c r="I6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="5">
         <v>0.1</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K6" s="5">
         <v>0.31</v>
       </c>
-      <c r="L6" s="6">
+      <c r="L6" s="5">
         <v>0.15</v>
       </c>
-      <c r="M6" s="6">
+      <c r="M6" s="5">
         <v>858</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+      <c r="A7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="8">
-        <v>0</v>
-      </c>
-      <c r="C7" s="8">
-        <v>0</v>
-      </c>
-      <c r="D7" s="8">
-        <v>0</v>
-      </c>
-      <c r="E7" s="12">
+      <c r="B7" s="7">
+        <v>0</v>
+      </c>
+      <c r="C7" s="7">
+        <v>0</v>
+      </c>
+      <c r="D7" s="7">
+        <v>0</v>
+      </c>
+      <c r="E7" s="10">
         <v>6112</v>
       </c>
-      <c r="F7" s="8"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
-      <c r="I7" s="8" t="s">
+      <c r="F7" s="7"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="J7" s="8">
+      <c r="J7" s="7">
         <v>0.77</v>
       </c>
-      <c r="K7" s="8">
+      <c r="K7" s="7">
         <v>0.03</v>
       </c>
-      <c r="L7" s="8">
+      <c r="L7" s="7">
         <v>0.06</v>
       </c>
-      <c r="M7" s="12">
+      <c r="M7" s="10">
         <v>6111</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>0.43</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>0.87</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>0.57999999999999996</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="8">
         <v>5872</v>
       </c>
-      <c r="F8" s="6"/>
-      <c r="I8" s="6" t="s">
+      <c r="F8" s="5"/>
+      <c r="I8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J8" s="5">
         <v>0.43</v>
       </c>
-      <c r="K8" s="6">
+      <c r="K8" s="5">
         <v>0.86</v>
       </c>
-      <c r="L8" s="6">
+      <c r="L8" s="5">
         <v>0.57999999999999996</v>
       </c>
-      <c r="M8" s="10">
+      <c r="M8" s="8">
         <v>5980</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>0.37</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>0.45</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>0.41</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>882</v>
       </c>
-      <c r="F9" s="6"/>
-      <c r="I9" s="6" t="s">
+      <c r="F9" s="5"/>
+      <c r="I9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="5">
         <v>0.36</v>
       </c>
-      <c r="K9" s="6">
+      <c r="K9" s="5">
         <v>0.45</v>
       </c>
-      <c r="L9" s="6">
+      <c r="L9" s="5">
         <v>0.4</v>
       </c>
-      <c r="M9" s="6">
+      <c r="M9" s="5">
         <v>937</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>0.6</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>0.62</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <v>0.61</v>
       </c>
-      <c r="E10" s="10">
+      <c r="E10" s="8">
         <v>3356</v>
       </c>
-      <c r="F10" s="8"/>
-      <c r="I10" s="6" t="s">
+      <c r="F10" s="7"/>
+      <c r="I10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="J10" s="6">
+      <c r="J10" s="5">
         <v>0.62</v>
       </c>
-      <c r="K10" s="6">
+      <c r="K10" s="5">
         <v>0.59</v>
       </c>
-      <c r="L10" s="6">
+      <c r="L10" s="5">
         <v>0.6</v>
       </c>
-      <c r="M10" s="10">
+      <c r="M10" s="8">
         <v>3467</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="6">
-        <v>0</v>
-      </c>
-      <c r="C11" s="6">
-        <v>0</v>
-      </c>
-      <c r="D11" s="6">
-        <v>0</v>
-      </c>
-      <c r="E11" s="6">
+      <c r="B11" s="5">
+        <v>0</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0</v>
+      </c>
+      <c r="E11" s="5">
         <v>433</v>
       </c>
-      <c r="F11" s="6"/>
-      <c r="I11" s="6" t="s">
+      <c r="F11" s="5"/>
+      <c r="I11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="6">
-        <v>0</v>
-      </c>
-      <c r="K11" s="6">
-        <v>0</v>
-      </c>
-      <c r="L11" s="6">
-        <v>0</v>
-      </c>
-      <c r="M11" s="6">
+      <c r="J11" s="5">
+        <v>0</v>
+      </c>
+      <c r="K11" s="5">
+        <v>0</v>
+      </c>
+      <c r="L11" s="5">
+        <v>0</v>
+      </c>
+      <c r="M11" s="5">
         <v>374</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="6">
-        <v>0</v>
-      </c>
-      <c r="C12" s="6">
-        <v>0</v>
-      </c>
-      <c r="D12" s="6">
-        <v>0</v>
-      </c>
-      <c r="E12" s="6">
+      <c r="B12" s="5">
+        <v>0</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0</v>
+      </c>
+      <c r="E12" s="5">
         <v>48</v>
       </c>
-      <c r="F12" s="6"/>
-      <c r="I12" s="6" t="s">
+      <c r="F12" s="5"/>
+      <c r="I12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="J12" s="6">
-        <v>0</v>
-      </c>
-      <c r="K12" s="6">
-        <v>0</v>
-      </c>
-      <c r="L12" s="6">
-        <v>0</v>
-      </c>
-      <c r="M12" s="6">
+      <c r="J12" s="5">
+        <v>0</v>
+      </c>
+      <c r="K12" s="5">
+        <v>0</v>
+      </c>
+      <c r="L12" s="5">
+        <v>0</v>
+      </c>
+      <c r="M12" s="5">
         <v>54</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B13" s="6"/>
-      <c r="C13" s="6"/>
-      <c r="D13" s="7">
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="6">
         <v>0.87</v>
       </c>
-      <c r="E13" s="11">
+      <c r="E13" s="9">
         <v>89583</v>
       </c>
-      <c r="F13" s="6"/>
-      <c r="I13" s="7" t="s">
+      <c r="F13" s="5"/>
+      <c r="I13" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="J13" s="6"/>
-      <c r="K13" s="6"/>
-      <c r="L13" s="7">
+      <c r="J13" s="5"/>
+      <c r="K13" s="5"/>
+      <c r="L13" s="6">
         <v>0.87</v>
       </c>
-      <c r="M13" s="11">
+      <c r="M13" s="9">
         <v>89583</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="5">
         <v>0.34</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <v>0.33</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="5">
         <v>0.28999999999999998</v>
       </c>
-      <c r="E14" s="10">
+      <c r="E14" s="8">
         <v>89583</v>
       </c>
-      <c r="F14" s="6"/>
-      <c r="I14" s="7" t="s">
+      <c r="F14" s="5"/>
+      <c r="I14" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="J14" s="6">
+      <c r="J14" s="5">
         <v>0.4</v>
       </c>
-      <c r="K14" s="6">
+      <c r="K14" s="5">
         <v>0.33</v>
       </c>
-      <c r="L14" s="6">
+      <c r="L14" s="5">
         <v>0.28999999999999998</v>
       </c>
-      <c r="M14" s="10">
+      <c r="M14" s="8">
         <v>89583</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B15" s="6">
+      <c r="B15" s="5">
         <v>0.85</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15" s="5">
         <v>0.87</v>
       </c>
-      <c r="D15" s="6">
+      <c r="D15" s="5">
         <v>0.85</v>
       </c>
-      <c r="E15" s="10">
+      <c r="E15" s="8">
         <v>89583</v>
       </c>
-      <c r="I15" s="7" t="s">
+      <c r="I15" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="J15" s="6">
+      <c r="J15" s="5">
         <v>0.91</v>
       </c>
-      <c r="K15" s="6">
+      <c r="K15" s="5">
         <v>0.87</v>
       </c>
-      <c r="L15" s="6">
+      <c r="L15" s="5">
         <v>0.86</v>
       </c>
-      <c r="M15" s="10">
+      <c r="M15" s="8">
         <v>89583</v>
       </c>
     </row>
     <row r="17" spans="1:13" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="14" t="s">
+      <c r="A17" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B17" s="14"/>
-      <c r="C17" s="14"/>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14"/>
-      <c r="F17" s="14"/>
-      <c r="G17" s="14"/>
-      <c r="H17" s="14"/>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
-      <c r="K17" s="14"/>
-      <c r="L17" s="14"/>
-      <c r="M17" s="14"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="22"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="22"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="22"/>
+      <c r="J17" s="22"/>
+      <c r="K17" s="22"/>
+      <c r="L17" s="22"/>
+      <c r="M17" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2054,311 +2090,311 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="9" t="s">
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="23"/>
+      <c r="E1" s="23"/>
+      <c r="F1" s="23"/>
+      <c r="G1" s="3"/>
+      <c r="H1" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="I1" s="9"/>
+      <c r="I1" s="23"/>
     </row>
     <row r="2" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="6">
-        <v>0</v>
-      </c>
-      <c r="C3" s="6">
-        <v>0</v>
-      </c>
-      <c r="D3" s="6">
-        <v>0</v>
-      </c>
-      <c r="E3" s="6">
+      <c r="B3" s="5">
+        <v>0</v>
+      </c>
+      <c r="C3" s="5">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5">
+        <v>0</v>
+      </c>
+      <c r="E3" s="5">
         <v>75</v>
       </c>
-      <c r="F3" s="6"/>
-      <c r="H3" s="6" t="s">
+      <c r="F3" s="5"/>
+      <c r="H3" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="5">
         <v>0.94906299999999999</v>
       </c>
     </row>
     <row r="4" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="6">
-        <v>0</v>
-      </c>
-      <c r="C4" s="6">
-        <v>0</v>
-      </c>
-      <c r="D4" s="6">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6">
+      <c r="B4" s="5">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5">
         <v>90</v>
       </c>
-      <c r="F4" s="6"/>
-      <c r="H4" s="6" t="s">
+      <c r="F4" s="5"/>
+      <c r="H4" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="I4" s="6">
+      <c r="I4" s="5">
         <v>0.99424299999999999</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>0.999448</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>0.97353699999999999</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>0.98632200000000003</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>71591</v>
       </c>
-      <c r="F5" s="6"/>
-      <c r="H5" s="6" t="s">
+      <c r="F5" s="5"/>
+      <c r="H5" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="5">
         <v>0.969495</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>0.92857100000000004</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>8.0370000000000007E-3</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>1.5935000000000001E-2</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>871</v>
       </c>
-      <c r="F6" s="6"/>
-      <c r="H6" s="6" t="s">
+      <c r="F6" s="5"/>
+      <c r="H6" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="5">
         <v>0.90797099999999997</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>0.74248499999999995</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>0.66434199999999999</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>0.70117799999999997</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>6237</v>
       </c>
-      <c r="F7" s="6"/>
-      <c r="H7" s="6" t="s">
+      <c r="F7" s="5"/>
+      <c r="H7" s="5" t="s">
         <v>18</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="5">
         <v>0.99410799999999999</v>
       </c>
     </row>
     <row r="8" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>0.49457899999999999</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>0.933755</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>0.64664900000000003</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>6008</v>
       </c>
-      <c r="F8" s="6"/>
-      <c r="H8" s="6" t="s">
+      <c r="F8" s="5"/>
+      <c r="H8" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="5">
         <v>2.5337999999999999E-2</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="45" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>0.84633499999999995</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>0.326206</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>0.470885</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>912</v>
       </c>
-      <c r="F9" s="6"/>
-      <c r="H9" s="6" t="s">
+      <c r="F9" s="5"/>
+      <c r="H9" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="5">
         <v>5.8919999999999997E-3</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>0.80440900000000004</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>0.61624800000000002</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <v>0.69738900000000004</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>3342</v>
       </c>
-      <c r="F10" s="6"/>
+      <c r="F10" s="5"/>
     </row>
     <row r="11" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="6">
-        <v>0</v>
-      </c>
-      <c r="C11" s="6">
-        <v>0</v>
-      </c>
-      <c r="D11" s="6">
-        <v>0</v>
-      </c>
-      <c r="E11" s="6">
+      <c r="B11" s="5">
+        <v>0</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0</v>
+      </c>
+      <c r="E11" s="5">
         <v>413</v>
       </c>
-      <c r="F11" s="6"/>
+      <c r="F11" s="5"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="6">
-        <v>0</v>
-      </c>
-      <c r="C12" s="6">
-        <v>0</v>
-      </c>
-      <c r="D12" s="6">
-        <v>0</v>
-      </c>
-      <c r="E12" s="6">
+      <c r="B12" s="5">
+        <v>0</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0</v>
+      </c>
+      <c r="E12" s="5">
         <v>44</v>
       </c>
-      <c r="F12" s="6"/>
+      <c r="F12" s="5"/>
     </row>
     <row r="13" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>0.48158299999999998</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <v>0.35221200000000003</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="5">
         <v>0.35183599999999998</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <v>89583</v>
       </c>
-      <c r="F13" s="6"/>
+      <c r="F13" s="5"/>
     </row>
     <row r="14" spans="1:9" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="5">
         <v>0.93123400000000001</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <v>0.91327599999999998</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="5">
         <v>0.91137999999999997</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="5">
         <v>89583</v>
       </c>
-      <c r="F14" s="6"/>
+      <c r="F14" s="5"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="5" t="s">
+      <c r="A15" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="9">
+      <c r="B15" s="23">
         <v>0.91327599999999998</v>
       </c>
-      <c r="C15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
+      <c r="C15" s="23"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -2381,667 +2417,667 @@
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:19" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="15" t="s">
+      <c r="A1" s="24" t="s">
         <v>41</v>
       </c>
-      <c r="B1" s="15"/>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="H1" s="15" t="s">
+      <c r="B1" s="24"/>
+      <c r="C1" s="24"/>
+      <c r="D1" s="24"/>
+      <c r="E1" s="24"/>
+      <c r="H1" s="24" t="s">
         <v>26</v>
       </c>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="O1" s="15" t="s">
+      <c r="I1" s="24"/>
+      <c r="J1" s="24"/>
+      <c r="K1" s="24"/>
+      <c r="L1" s="24"/>
+      <c r="O1" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="P1" s="15"/>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="15"/>
+      <c r="P1" s="24"/>
+      <c r="Q1" s="24"/>
+      <c r="R1" s="24"/>
+      <c r="S1" s="24"/>
     </row>
     <row r="2" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="5" t="s">
+      <c r="E2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="H2" s="5" t="s">
+      <c r="H2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="J2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="K2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="L2" s="5" t="s">
+      <c r="L2" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="P2" s="5" t="s">
+      <c r="P2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="Q2" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="R2" s="5" t="s">
+      <c r="R2" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="S2" s="4" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="6">
+      <c r="B3" s="5">
         <v>1</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="5">
         <v>0.97</v>
       </c>
-      <c r="D3" s="6">
+      <c r="D3" s="5">
         <v>0.99</v>
       </c>
-      <c r="E3" s="6">
+      <c r="E3" s="5">
         <v>71593</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="I3" s="6">
+      <c r="I3" s="5">
         <v>1</v>
       </c>
-      <c r="J3" s="6">
+      <c r="J3" s="5">
         <v>0.97</v>
       </c>
-      <c r="K3" s="6">
+      <c r="K3" s="5">
         <v>0.98</v>
       </c>
-      <c r="L3" s="6">
+      <c r="L3" s="5">
         <v>71681</v>
       </c>
-      <c r="O3" s="6" t="s">
+      <c r="O3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="P3" s="6">
+      <c r="P3" s="5">
         <v>1</v>
       </c>
-      <c r="Q3" s="6">
+      <c r="Q3" s="5">
         <v>0.97</v>
       </c>
-      <c r="R3" s="6">
+      <c r="R3" s="5">
         <v>0.99</v>
       </c>
-      <c r="S3" s="6">
+      <c r="S3" s="5">
         <v>71464</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="A4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="6">
-        <v>0</v>
-      </c>
-      <c r="C4" s="6">
-        <v>0</v>
-      </c>
-      <c r="D4" s="6">
-        <v>0</v>
-      </c>
-      <c r="E4" s="6">
+      <c r="B4" s="5">
+        <v>0</v>
+      </c>
+      <c r="C4" s="5">
+        <v>0</v>
+      </c>
+      <c r="D4" s="5">
+        <v>0</v>
+      </c>
+      <c r="E4" s="5">
         <v>84</v>
       </c>
-      <c r="H4" s="6" t="s">
+      <c r="H4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="I4" s="6">
-        <v>0</v>
-      </c>
-      <c r="J4" s="6">
-        <v>0</v>
-      </c>
-      <c r="K4" s="6">
-        <v>0</v>
-      </c>
-      <c r="L4" s="6">
+      <c r="I4" s="5">
+        <v>0</v>
+      </c>
+      <c r="J4" s="5">
+        <v>0</v>
+      </c>
+      <c r="K4" s="5">
+        <v>0</v>
+      </c>
+      <c r="L4" s="5">
         <v>81</v>
       </c>
-      <c r="O4" s="6" t="s">
+      <c r="O4" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="P4" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q4" s="6">
-        <v>0</v>
-      </c>
-      <c r="R4" s="6">
-        <v>0</v>
-      </c>
-      <c r="S4" s="6">
+      <c r="P4" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>0</v>
+      </c>
+      <c r="R4" s="5">
+        <v>0</v>
+      </c>
+      <c r="S4" s="5">
         <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
+      <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="6">
+      <c r="B5" s="5">
         <v>0.8</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="5">
         <v>0.05</v>
       </c>
-      <c r="D5" s="6">
+      <c r="D5" s="5">
         <v>0.09</v>
       </c>
-      <c r="E5" s="6">
+      <c r="E5" s="5">
         <v>83</v>
       </c>
-      <c r="H5" s="6" t="s">
+      <c r="H5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="I5" s="6">
+      <c r="I5" s="5">
         <v>1</v>
       </c>
-      <c r="J5" s="6">
+      <c r="J5" s="5">
         <v>0.06</v>
       </c>
-      <c r="K5" s="6">
+      <c r="K5" s="5">
         <v>0.12</v>
       </c>
-      <c r="L5" s="6">
+      <c r="L5" s="5">
         <v>97</v>
       </c>
-      <c r="O5" s="6" t="s">
+      <c r="O5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="P5" s="6">
+      <c r="P5" s="5">
         <v>0.56999999999999995</v>
       </c>
-      <c r="Q5" s="6">
+      <c r="Q5" s="5">
         <v>0.04</v>
       </c>
-      <c r="R5" s="6">
+      <c r="R5" s="5">
         <v>0.08</v>
       </c>
-      <c r="S5" s="6">
+      <c r="S5" s="5">
         <v>96</v>
       </c>
     </row>
     <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="A6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="6">
+      <c r="B6" s="5">
         <v>0.52</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="5">
         <v>0.02</v>
       </c>
-      <c r="D6" s="6">
+      <c r="D6" s="5">
         <v>0.03</v>
       </c>
-      <c r="E6" s="6">
+      <c r="E6" s="5">
         <v>882</v>
       </c>
-      <c r="H6" s="6" t="s">
+      <c r="H6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="I6" s="6">
+      <c r="I6" s="5">
         <v>0.6</v>
       </c>
-      <c r="J6" s="6">
+      <c r="J6" s="5">
         <v>0.02</v>
       </c>
-      <c r="K6" s="6">
+      <c r="K6" s="5">
         <v>0.04</v>
       </c>
-      <c r="L6" s="6">
+      <c r="L6" s="5">
         <v>916</v>
       </c>
-      <c r="O6" s="6" t="s">
+      <c r="O6" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="P6" s="6">
+      <c r="P6" s="5">
         <v>0.53</v>
       </c>
-      <c r="Q6" s="6">
+      <c r="Q6" s="5">
         <v>0.02</v>
       </c>
-      <c r="R6" s="6">
+      <c r="R6" s="5">
         <v>0.04</v>
       </c>
-      <c r="S6" s="6">
+      <c r="S6" s="5">
         <v>886</v>
       </c>
     </row>
     <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
+      <c r="A7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B7" s="6">
+      <c r="B7" s="5">
         <v>0.7</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="5">
         <v>0.63</v>
       </c>
-      <c r="D7" s="6">
+      <c r="D7" s="5">
         <v>0.66</v>
       </c>
-      <c r="E7" s="6">
+      <c r="E7" s="5">
         <v>6232</v>
       </c>
-      <c r="H7" s="6" t="s">
+      <c r="H7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="I7" s="6">
+      <c r="I7" s="5">
         <v>0.69</v>
       </c>
-      <c r="J7" s="6">
+      <c r="J7" s="5">
         <v>0.62</v>
       </c>
-      <c r="K7" s="6">
+      <c r="K7" s="5">
         <v>0.66</v>
       </c>
-      <c r="L7" s="6">
+      <c r="L7" s="5">
         <v>6112</v>
       </c>
-      <c r="O7" s="6" t="s">
+      <c r="O7" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="P7" s="6">
+      <c r="P7" s="5">
         <v>0.69</v>
       </c>
-      <c r="Q7" s="6">
+      <c r="Q7" s="5">
         <v>0.62</v>
       </c>
-      <c r="R7" s="6">
+      <c r="R7" s="5">
         <v>0.65</v>
       </c>
-      <c r="S7" s="6">
+      <c r="S7" s="5">
         <v>6173</v>
       </c>
     </row>
     <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
+      <c r="A8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="B8" s="6">
+      <c r="B8" s="5">
         <v>0.44</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="5">
         <v>0.8</v>
       </c>
-      <c r="D8" s="6">
+      <c r="D8" s="5">
         <v>0.56999999999999995</v>
       </c>
-      <c r="E8" s="6">
+      <c r="E8" s="5">
         <v>5933</v>
       </c>
-      <c r="H8" s="6" t="s">
+      <c r="H8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="6">
+      <c r="I8" s="5">
         <v>0.45</v>
       </c>
-      <c r="J8" s="6">
+      <c r="J8" s="5">
         <v>0.8</v>
       </c>
-      <c r="K8" s="6">
+      <c r="K8" s="5">
         <v>0.56999999999999995</v>
       </c>
-      <c r="L8" s="6">
+      <c r="L8" s="5">
         <v>5989</v>
       </c>
-      <c r="O8" s="6" t="s">
+      <c r="O8" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="P8" s="6">
+      <c r="P8" s="5">
         <v>0.45</v>
       </c>
-      <c r="Q8" s="6">
+      <c r="Q8" s="5">
         <v>0.8</v>
       </c>
-      <c r="R8" s="6">
+      <c r="R8" s="5">
         <v>0.56999999999999995</v>
       </c>
-      <c r="S8" s="6">
+      <c r="S8" s="5">
         <v>6055</v>
       </c>
     </row>
     <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
+      <c r="A9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="6">
+      <c r="B9" s="5">
         <v>0.67</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="5">
         <v>0.2</v>
       </c>
-      <c r="D9" s="6">
+      <c r="D9" s="5">
         <v>0.31</v>
       </c>
-      <c r="E9" s="6">
+      <c r="E9" s="5">
         <v>976</v>
       </c>
-      <c r="H9" s="6" t="s">
+      <c r="H9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="I9" s="6">
+      <c r="I9" s="5">
         <v>0.66</v>
       </c>
-      <c r="J9" s="6">
+      <c r="J9" s="5">
         <v>0.21</v>
       </c>
-      <c r="K9" s="6">
+      <c r="K9" s="5">
         <v>0.32</v>
       </c>
-      <c r="L9" s="6">
+      <c r="L9" s="5">
         <v>912</v>
       </c>
-      <c r="O9" s="6" t="s">
+      <c r="O9" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="P9" s="6">
+      <c r="P9" s="5">
         <v>0.68</v>
       </c>
-      <c r="Q9" s="6">
+      <c r="Q9" s="5">
         <v>0.21</v>
       </c>
-      <c r="R9" s="6">
+      <c r="R9" s="5">
         <v>0.32</v>
       </c>
-      <c r="S9" s="6">
+      <c r="S9" s="5">
         <v>979</v>
       </c>
     </row>
     <row r="10" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="6" t="s">
+      <c r="A10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="6">
+      <c r="B10" s="5">
         <v>0.62</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="5">
         <v>0.55000000000000004</v>
       </c>
-      <c r="D10" s="6">
+      <c r="D10" s="5">
         <v>0.57999999999999996</v>
       </c>
-      <c r="E10" s="6">
+      <c r="E10" s="5">
         <v>3311</v>
       </c>
-      <c r="H10" s="6" t="s">
+      <c r="H10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="I10" s="6">
+      <c r="I10" s="5">
         <v>0.62</v>
       </c>
-      <c r="J10" s="6">
+      <c r="J10" s="5">
         <v>0.56999999999999995</v>
       </c>
-      <c r="K10" s="6">
+      <c r="K10" s="5">
         <v>0.6</v>
       </c>
-      <c r="L10" s="6">
+      <c r="L10" s="5">
         <v>3315</v>
       </c>
-      <c r="O10" s="6" t="s">
+      <c r="O10" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="P10" s="6">
+      <c r="P10" s="5">
         <v>0.62</v>
       </c>
-      <c r="Q10" s="6">
+      <c r="Q10" s="5">
         <v>0.57999999999999996</v>
       </c>
-      <c r="R10" s="6">
+      <c r="R10" s="5">
         <v>0.6</v>
       </c>
-      <c r="S10" s="6">
+      <c r="S10" s="5">
         <v>3324</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
+      <c r="A11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="6">
-        <v>0</v>
-      </c>
-      <c r="C11" s="6">
-        <v>0</v>
-      </c>
-      <c r="D11" s="6">
-        <v>0</v>
-      </c>
-      <c r="E11" s="6">
+      <c r="B11" s="5">
+        <v>0</v>
+      </c>
+      <c r="C11" s="5">
+        <v>0</v>
+      </c>
+      <c r="D11" s="5">
+        <v>0</v>
+      </c>
+      <c r="E11" s="5">
         <v>437</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="H11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="I11" s="6">
-        <v>0</v>
-      </c>
-      <c r="J11" s="6">
-        <v>0</v>
-      </c>
-      <c r="K11" s="6">
-        <v>0</v>
-      </c>
-      <c r="L11" s="6">
+      <c r="I11" s="5">
+        <v>0</v>
+      </c>
+      <c r="J11" s="5">
+        <v>0</v>
+      </c>
+      <c r="K11" s="5">
+        <v>0</v>
+      </c>
+      <c r="L11" s="5">
         <v>421</v>
       </c>
-      <c r="O11" s="6" t="s">
+      <c r="O11" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="P11" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q11" s="6">
-        <v>0</v>
-      </c>
-      <c r="R11" s="6">
-        <v>0</v>
-      </c>
-      <c r="S11" s="6">
+      <c r="P11" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q11" s="5">
+        <v>0</v>
+      </c>
+      <c r="R11" s="5">
+        <v>0</v>
+      </c>
+      <c r="S11" s="5">
         <v>453</v>
       </c>
     </row>
     <row r="12" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A12" s="6" t="s">
+      <c r="A12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="6">
-        <v>0</v>
-      </c>
-      <c r="C12" s="6">
-        <v>0</v>
-      </c>
-      <c r="D12" s="6">
-        <v>0</v>
-      </c>
-      <c r="E12" s="6">
+      <c r="B12" s="5">
+        <v>0</v>
+      </c>
+      <c r="C12" s="5">
+        <v>0</v>
+      </c>
+      <c r="D12" s="5">
+        <v>0</v>
+      </c>
+      <c r="E12" s="5">
         <v>52</v>
       </c>
-      <c r="H12" s="6" t="s">
+      <c r="H12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="I12" s="6">
-        <v>0</v>
-      </c>
-      <c r="J12" s="6">
-        <v>0</v>
-      </c>
-      <c r="K12" s="6">
-        <v>0</v>
-      </c>
-      <c r="L12" s="6">
+      <c r="I12" s="5">
+        <v>0</v>
+      </c>
+      <c r="J12" s="5">
+        <v>0</v>
+      </c>
+      <c r="K12" s="5">
+        <v>0</v>
+      </c>
+      <c r="L12" s="5">
         <v>59</v>
       </c>
-      <c r="O12" s="6" t="s">
+      <c r="O12" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="P12" s="6">
-        <v>0</v>
-      </c>
-      <c r="Q12" s="6">
-        <v>0</v>
-      </c>
-      <c r="R12" s="6">
-        <v>0</v>
-      </c>
-      <c r="S12" s="6">
+      <c r="P12" s="5">
+        <v>0</v>
+      </c>
+      <c r="Q12" s="5">
+        <v>0</v>
+      </c>
+      <c r="R12" s="5">
+        <v>0</v>
+      </c>
+      <c r="S12" s="5">
         <v>61</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="7" t="s">
+      <c r="A13" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="6">
+      <c r="B13" s="5">
         <v>0.47</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="5">
         <v>0.32</v>
       </c>
-      <c r="D13" s="6">
+      <c r="D13" s="5">
         <v>0.32</v>
       </c>
-      <c r="E13" s="6">
+      <c r="E13" s="5">
         <v>89583</v>
       </c>
-      <c r="H13" s="7" t="s">
+      <c r="H13" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="I13" s="6">
+      <c r="I13" s="5">
         <v>0.5</v>
       </c>
-      <c r="J13" s="6">
+      <c r="J13" s="5">
         <v>0.33</v>
       </c>
-      <c r="K13" s="6">
+      <c r="K13" s="5">
         <v>0.33</v>
       </c>
-      <c r="L13" s="6">
+      <c r="L13" s="5">
         <v>89583</v>
       </c>
-      <c r="O13" s="7" t="s">
+      <c r="O13" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="P13" s="6">
+      <c r="P13" s="5">
         <v>0.45</v>
       </c>
-      <c r="Q13" s="6">
+      <c r="Q13" s="5">
         <v>0.32</v>
       </c>
-      <c r="R13" s="6">
+      <c r="R13" s="5">
         <v>0.32</v>
       </c>
-      <c r="S13" s="6">
+      <c r="S13" s="5">
         <v>89583</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="7" t="s">
+      <c r="A14" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="6">
+      <c r="B14" s="5">
         <v>0.91</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="5">
         <v>0.9</v>
       </c>
-      <c r="D14" s="6">
+      <c r="D14" s="5">
         <v>0.9</v>
       </c>
-      <c r="E14" s="6">
+      <c r="E14" s="5">
         <v>89583</v>
       </c>
-      <c r="H14" s="7" t="s">
+      <c r="H14" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="I14" s="6">
+      <c r="I14" s="5">
         <v>0.91</v>
       </c>
-      <c r="J14" s="6">
+      <c r="J14" s="5">
         <v>0.9</v>
       </c>
-      <c r="K14" s="6">
+      <c r="K14" s="5">
         <v>0.9</v>
       </c>
-      <c r="L14" s="6">
+      <c r="L14" s="5">
         <v>89583</v>
       </c>
-      <c r="O14" s="7" t="s">
+      <c r="O14" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="P14" s="6">
+      <c r="P14" s="5">
         <v>0.91</v>
       </c>
-      <c r="Q14" s="6">
+      <c r="Q14" s="5">
         <v>0.9</v>
       </c>
-      <c r="R14" s="6">
+      <c r="R14" s="5">
         <v>0.9</v>
       </c>
-      <c r="S14" s="6">
+      <c r="S14" s="5">
         <v>89583</v>
       </c>
     </row>
     <row r="15" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A15" s="7" t="s">
+      <c r="A15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="B15" s="14">
+      <c r="B15" s="22">
         <v>0.9</v>
       </c>
-      <c r="C15" s="14"/>
-      <c r="D15" s="14"/>
-      <c r="E15" s="14"/>
-      <c r="H15" s="7" t="s">
+      <c r="C15" s="22"/>
+      <c r="D15" s="22"/>
+      <c r="E15" s="22"/>
+      <c r="H15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="I15" s="14">
+      <c r="I15" s="22">
         <v>0.9</v>
       </c>
-      <c r="J15" s="14"/>
-      <c r="K15" s="14"/>
-      <c r="L15" s="14"/>
-      <c r="O15" s="7" t="s">
+      <c r="J15" s="22"/>
+      <c r="K15" s="22"/>
+      <c r="L15" s="22"/>
+      <c r="O15" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="P15" s="14">
+      <c r="P15" s="22">
         <v>0.9</v>
       </c>
-      <c r="Q15" s="14"/>
-      <c r="R15" s="14"/>
-      <c r="S15" s="14"/>
+      <c r="Q15" s="22"/>
+      <c r="R15" s="22"/>
+      <c r="S15" s="22"/>
     </row>
   </sheetData>
   <mergeCells count="6">

</xml_diff>